<commit_message>
ref #13263 SDK Code sample & Testing - Test Contact
</commit_message>
<xml_diff>
--- a/SDK/RESULT/ReportCheckAPI_v2.xlsx
+++ b/SDK/RESULT/ReportCheckAPI_v2.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="2" r:id="rId1"/>
     <sheet name="Success" sheetId="3" r:id="rId2"/>
     <sheet name="Fail" sheetId="4" r:id="rId3"/>
     <sheet name="Not implement" sheetId="5" r:id="rId4"/>
+    <sheet name="NamNguyen-10152014" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="104">
   <si>
     <t>STT</t>
   </si>
@@ -845,13 +841,130 @@
   </si>
   <si>
     <t>Intent ,don't understand function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Method and Description </t>
+  </si>
+  <si>
+    <t>Modifier and  Type</t>
+  </si>
+  <si>
+    <t>fetch();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact[] </t>
+  </si>
+  <si>
+    <t>fetch(47, false);</t>
+  </si>
+  <si>
+    <t>- Run</t>
+  </si>
+  <si>
+    <t>fetch("979485576",false);</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>verifyNumber("+84979485576");</t>
+  </si>
+  <si>
+    <t>addContactListener(IOnSyncContactsListener listener);</t>
+  </si>
+  <si>
+    <t>checkForChanges();</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Run </t>
+  </si>
+  <si>
+    <t>List&lt;String&gt;</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bitmap </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fail </t>
+  </si>
+  <si>
+    <t xml:space="preserve">String </t>
+  </si>
+  <si>
+    <t>Bitmap</t>
+  </si>
+  <si>
+    <t>List&lt;com.voipswitch.contacts.Contact.Phone&gt;</t>
+  </si>
+  <si>
+    <t>isVippieId(java.lang.String number);</t>
+  </si>
+  <si>
+    <t>isVippieNumber(java.lang.String number);</t>
+  </si>
+  <si>
+    <t>hasVippieNumber(java.util.List&lt;com.voipswitch.contacts.Contact.Phone&gt; list);</t>
+  </si>
+  <si>
+    <t>getVippieLoginForNumber(java.lang.String number);</t>
+  </si>
+  <si>
+    <t>getNumberForVippie(java.lang.String number);</t>
+  </si>
+  <si>
+    <t>getContactPhoto(com.voipswitch.contacts.Contact.Phone phone, unique.packagename.util.IImageRepository.IImageRepositoryCallback&lt;com.voipswitch.contacts.Contact.Phone&gt; callback);</t>
+  </si>
+  <si>
+    <t>containsVippieNumbersCached(java.util.List&lt;com.voipswitch.contacts.Contact.Phone&gt; list);</t>
+  </si>
+  <si>
+    <t>containsVippieNumber(java.util.List&lt;com.voipswitch.contacts.Contact.Phone&gt; list);</t>
+  </si>
+  <si>
+    <t>getVippiePhones(java.util.List&lt;com.voipswitch.contacts.Contact.Phone&gt; list);</t>
+  </si>
+  <si>
+    <t>prepareNumber(java.lang.String number);</t>
+  </si>
+  <si>
+    <t>removeContactListener(IOnSyncContactsListener listener);</t>
+  </si>
+  <si>
+    <t>requestAddNew();</t>
+  </si>
+  <si>
+    <t>Intent</t>
+  </si>
+  <si>
+    <t>requestEdit(Contact contact);</t>
+  </si>
+  <si>
+    <t>requestView(Contact contact);</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>Note :</t>
+  </si>
+  <si>
+    <t>Not call onSipContactsSyncInited and onSynchronizedContactsChanged(String arg0).</t>
+  </si>
+  <si>
+    <t>How to used Check for change ? Why used ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -922,6 +1035,30 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1003,7 +1140,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1082,6 +1219,60 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1093,6 +1284,55 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1155,7 +1395,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1190,7 +1430,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1367,32 +1607,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="48.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="107.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="125.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="55.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="99.42578125" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1412,11 +1652,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="21" customHeight="1">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="46" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1430,11 +1670,11 @@
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="17.25" customHeight="1">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="47"/>
       <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
@@ -1446,11 +1686,11 @@
       </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="17.25" customHeight="1">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="47"/>
       <c r="C4" s="4" t="s">
         <v>16</v>
       </c>
@@ -1462,11 +1702,11 @@
       </c>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="17.25" customHeight="1">
       <c r="A5" s="9">
         <v>4</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="47"/>
       <c r="C5" s="10" t="s">
         <v>10</v>
       </c>
@@ -1478,11 +1718,11 @@
       </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="17.25" customHeight="1">
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="29"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
@@ -1494,11 +1734,11 @@
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="17.25" customHeight="1">
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="29"/>
+      <c r="B7" s="47"/>
       <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
@@ -1510,11 +1750,11 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="17.25" customHeight="1">
       <c r="A8" s="12">
         <v>7</v>
       </c>
-      <c r="B8" s="29"/>
+      <c r="B8" s="47"/>
       <c r="C8" s="13" t="s">
         <v>13</v>
       </c>
@@ -1526,11 +1766,11 @@
       </c>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="17.25" customHeight="1">
       <c r="A9" s="12">
         <v>8</v>
       </c>
-      <c r="B9" s="29"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="15" t="s">
         <v>12</v>
       </c>
@@ -1542,11 +1782,11 @@
       </c>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="17.25" customHeight="1">
       <c r="A10" s="9">
         <v>9</v>
       </c>
-      <c r="B10" s="30"/>
+      <c r="B10" s="48"/>
       <c r="C10" s="10" t="s">
         <v>11</v>
       </c>
@@ -1558,11 +1798,11 @@
       </c>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="33">
       <c r="A11" s="26">
         <v>10</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="46" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="16" t="s">
@@ -1576,11 +1816,11 @@
       </c>
       <c r="F11" s="25"/>
     </row>
-    <row r="12" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="27" customHeight="1">
       <c r="A12" s="26">
         <v>11</v>
       </c>
-      <c r="B12" s="29"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="17" t="s">
         <v>30</v>
       </c>
@@ -1592,11 +1832,11 @@
       </c>
       <c r="F12" s="25"/>
     </row>
-    <row r="13" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="33">
       <c r="A13" s="26">
         <v>12</v>
       </c>
-      <c r="B13" s="29"/>
+      <c r="B13" s="47"/>
       <c r="C13" s="17" t="s">
         <v>31</v>
       </c>
@@ -1608,11 +1848,11 @@
       </c>
       <c r="F13" s="25"/>
     </row>
-    <row r="14" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="33">
       <c r="A14" s="26">
         <v>13</v>
       </c>
-      <c r="B14" s="29"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="17" t="s">
         <v>32</v>
       </c>
@@ -1624,11 +1864,11 @@
       </c>
       <c r="F14" s="25"/>
     </row>
-    <row r="15" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="33">
       <c r="A15" s="26">
         <v>14</v>
       </c>
-      <c r="B15" s="29"/>
+      <c r="B15" s="47"/>
       <c r="C15" s="17" t="s">
         <v>33</v>
       </c>
@@ -1640,11 +1880,11 @@
       </c>
       <c r="F15" s="25"/>
     </row>
-    <row r="16" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="33">
       <c r="A16" s="26">
         <v>15</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="17" t="s">
         <v>34</v>
       </c>
@@ -1656,11 +1896,11 @@
       </c>
       <c r="F16" s="25"/>
     </row>
-    <row r="17" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="33">
       <c r="A17" s="26">
         <v>16</v>
       </c>
-      <c r="B17" s="29"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="17" t="s">
         <v>35</v>
       </c>
@@ -1672,11 +1912,11 @@
       </c>
       <c r="F17" s="25"/>
     </row>
-    <row r="18" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="49.5">
       <c r="A18" s="26">
         <v>17</v>
       </c>
-      <c r="B18" s="29"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="17" t="s">
         <v>36</v>
       </c>
@@ -1688,11 +1928,11 @@
       </c>
       <c r="F18" s="25"/>
     </row>
-    <row r="19" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="49.5">
       <c r="A19" s="26">
         <v>18</v>
       </c>
-      <c r="B19" s="29"/>
+      <c r="B19" s="47"/>
       <c r="C19" s="17" t="s">
         <v>37</v>
       </c>
@@ -1704,11 +1944,11 @@
       </c>
       <c r="F19" s="25"/>
     </row>
-    <row r="20" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="33">
       <c r="A20" s="26">
         <v>19</v>
       </c>
-      <c r="B20" s="29"/>
+      <c r="B20" s="47"/>
       <c r="C20" s="17" t="s">
         <v>38</v>
       </c>
@@ -1720,11 +1960,11 @@
       </c>
       <c r="F20" s="25"/>
     </row>
-    <row r="21" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="33">
       <c r="A21" s="26">
         <v>20</v>
       </c>
-      <c r="B21" s="29"/>
+      <c r="B21" s="47"/>
       <c r="C21" s="17" t="s">
         <v>39</v>
       </c>
@@ -1736,11 +1976,11 @@
       </c>
       <c r="F21" s="25"/>
     </row>
-    <row r="22" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="33">
       <c r="A22" s="26">
         <v>21</v>
       </c>
-      <c r="B22" s="29"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="17" t="s">
         <v>40</v>
       </c>
@@ -1752,11 +1992,11 @@
       </c>
       <c r="F22" s="25"/>
     </row>
-    <row r="23" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="33">
       <c r="A23" s="26">
         <v>22</v>
       </c>
-      <c r="B23" s="29"/>
+      <c r="B23" s="47"/>
       <c r="C23" s="17" t="s">
         <v>41</v>
       </c>
@@ -1768,11 +2008,11 @@
       </c>
       <c r="F23" s="25"/>
     </row>
-    <row r="24" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="33">
       <c r="A24" s="26">
         <v>23</v>
       </c>
-      <c r="B24" s="29"/>
+      <c r="B24" s="47"/>
       <c r="C24" s="17" t="s">
         <v>42</v>
       </c>
@@ -1784,11 +2024,11 @@
       </c>
       <c r="F24" s="25"/>
     </row>
-    <row r="25" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="33">
       <c r="A25" s="26">
         <v>24</v>
       </c>
-      <c r="B25" s="29"/>
+      <c r="B25" s="47"/>
       <c r="C25" s="17" t="s">
         <v>43</v>
       </c>
@@ -1800,11 +2040,11 @@
       </c>
       <c r="F25" s="25"/>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15" customHeight="1">
       <c r="A26" s="26">
         <v>25</v>
       </c>
-      <c r="B26" s="29"/>
+      <c r="B26" s="47"/>
       <c r="C26" s="21" t="s">
         <v>28</v>
       </c>
@@ -1816,11 +2056,11 @@
       </c>
       <c r="F26" s="25"/>
     </row>
-    <row r="27" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="49.5">
       <c r="A27" s="26">
         <v>26</v>
       </c>
-      <c r="B27" s="29"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="22" t="s">
         <v>44</v>
       </c>
@@ -1832,11 +2072,11 @@
       </c>
       <c r="F27" s="25"/>
     </row>
-    <row r="28" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="33">
       <c r="A28" s="26">
         <v>27</v>
       </c>
-      <c r="B28" s="29"/>
+      <c r="B28" s="47"/>
       <c r="C28" s="23" t="s">
         <v>45</v>
       </c>
@@ -1848,11 +2088,11 @@
       </c>
       <c r="F28" s="25"/>
     </row>
-    <row r="29" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="33">
       <c r="A29" s="26">
         <v>28</v>
       </c>
-      <c r="B29" s="29"/>
+      <c r="B29" s="47"/>
       <c r="C29" s="16" t="s">
         <v>46</v>
       </c>
@@ -1864,11 +2104,11 @@
       </c>
       <c r="F29" s="25"/>
     </row>
-    <row r="30" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="33">
       <c r="A30" s="26">
         <v>29</v>
       </c>
-      <c r="B30" s="29"/>
+      <c r="B30" s="47"/>
       <c r="C30" s="22" t="s">
         <v>47</v>
       </c>
@@ -1880,11 +2120,11 @@
       </c>
       <c r="F30" s="25"/>
     </row>
-    <row r="31" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="33">
       <c r="A31" s="26">
         <v>30</v>
       </c>
-      <c r="B31" s="29"/>
+      <c r="B31" s="47"/>
       <c r="C31" s="16" t="s">
         <v>48</v>
       </c>
@@ -1896,11 +2136,11 @@
       </c>
       <c r="F31" s="25"/>
     </row>
-    <row r="32" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="33">
       <c r="A32" s="26">
         <v>31</v>
       </c>
-      <c r="B32" s="29"/>
+      <c r="B32" s="47"/>
       <c r="C32" s="17" t="s">
         <v>49</v>
       </c>
@@ -1912,11 +2152,11 @@
       </c>
       <c r="F32" s="25"/>
     </row>
-    <row r="33" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="33">
       <c r="A33" s="26">
         <v>32</v>
       </c>
-      <c r="B33" s="29"/>
+      <c r="B33" s="47"/>
       <c r="C33" s="16" t="s">
         <v>50</v>
       </c>
@@ -1928,11 +2168,11 @@
       </c>
       <c r="F33" s="25"/>
     </row>
-    <row r="34" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="33">
       <c r="A34" s="26">
         <v>33</v>
       </c>
-      <c r="B34" s="29"/>
+      <c r="B34" s="47"/>
       <c r="C34" s="16" t="s">
         <v>51</v>
       </c>
@@ -1944,11 +2184,11 @@
       </c>
       <c r="F34" s="25"/>
     </row>
-    <row r="35" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="33">
       <c r="A35" s="26">
         <v>34</v>
       </c>
-      <c r="B35" s="30"/>
+      <c r="B35" s="48"/>
       <c r="C35" s="17" t="s">
         <v>52</v>
       </c>
@@ -1960,11 +2200,11 @@
       </c>
       <c r="F35" s="25"/>
     </row>
-    <row r="36" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="33">
       <c r="A36" s="26">
         <v>35</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="46" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="24" t="s">
@@ -1978,11 +2218,11 @@
       </c>
       <c r="F36" s="25"/>
     </row>
-    <row r="37" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="33">
       <c r="A37" s="26">
         <v>36</v>
       </c>
-      <c r="B37" s="29"/>
+      <c r="B37" s="47"/>
       <c r="C37" s="7" t="s">
         <v>54</v>
       </c>
@@ -1994,11 +2234,11 @@
       </c>
       <c r="F37" s="25"/>
     </row>
-    <row r="38" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="33">
       <c r="A38" s="26">
         <v>37</v>
       </c>
-      <c r="B38" s="29"/>
+      <c r="B38" s="47"/>
       <c r="C38" s="7" t="s">
         <v>55</v>
       </c>
@@ -2010,11 +2250,11 @@
       </c>
       <c r="F38" s="25"/>
     </row>
-    <row r="39" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="33">
       <c r="A39" s="26">
         <v>38</v>
       </c>
-      <c r="B39" s="30"/>
+      <c r="B39" s="48"/>
       <c r="C39" s="24" t="s">
         <v>56</v>
       </c>
@@ -2043,14 +2283,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="48.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -2061,7 +2301,7 @@
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2081,11 +2321,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="A2" s="3">
         <v>2</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="46" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -2099,11 +2339,11 @@
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="17.25" customHeight="1">
       <c r="A3" s="9">
         <v>4</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="47"/>
       <c r="C3" s="10" t="s">
         <v>10</v>
       </c>
@@ -2115,11 +2355,11 @@
       </c>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="17.25" customHeight="1">
       <c r="A4" s="3">
         <v>5</v>
       </c>
-      <c r="B4" s="30"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
@@ -2131,11 +2371,11 @@
       </c>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="33">
       <c r="A5" s="26">
         <v>10</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="46" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="16" t="s">
@@ -2149,11 +2389,11 @@
       </c>
       <c r="F5" s="25"/>
     </row>
-    <row r="6" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="33">
       <c r="A6" s="26">
         <v>11</v>
       </c>
-      <c r="B6" s="29"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="17" t="s">
         <v>30</v>
       </c>
@@ -2165,11 +2405,11 @@
       </c>
       <c r="F6" s="25"/>
     </row>
-    <row r="7" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="49.5">
       <c r="A7" s="26">
         <v>14</v>
       </c>
-      <c r="B7" s="29"/>
+      <c r="B7" s="47"/>
       <c r="C7" s="17" t="s">
         <v>33</v>
       </c>
@@ -2181,11 +2421,11 @@
       </c>
       <c r="F7" s="25"/>
     </row>
-    <row r="8" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="33">
       <c r="A8" s="26">
         <v>16</v>
       </c>
-      <c r="B8" s="29"/>
+      <c r="B8" s="47"/>
       <c r="C8" s="17" t="s">
         <v>35</v>
       </c>
@@ -2197,11 +2437,11 @@
       </c>
       <c r="F8" s="25"/>
     </row>
-    <row r="9" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="49.5">
       <c r="A9" s="26">
         <v>26</v>
       </c>
-      <c r="B9" s="29"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="22" t="s">
         <v>44</v>
       </c>
@@ -2213,11 +2453,11 @@
       </c>
       <c r="F9" s="25"/>
     </row>
-    <row r="10" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="33">
       <c r="A10" s="26">
         <v>34</v>
       </c>
-      <c r="B10" s="30"/>
+      <c r="B10" s="48"/>
       <c r="C10" s="17" t="s">
         <v>52</v>
       </c>
@@ -2229,7 +2469,7 @@
       </c>
       <c r="F10" s="25"/>
     </row>
-    <row r="11" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="33">
       <c r="A11" s="26">
         <v>38</v>
       </c>
@@ -2262,14 +2502,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="48.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -2280,7 +2520,7 @@
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2300,11 +2540,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1">
       <c r="A2" s="12">
         <v>7</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="47" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -2318,11 +2558,11 @@
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="17.25" customHeight="1">
       <c r="A3" s="9">
         <v>9</v>
       </c>
-      <c r="B3" s="30"/>
+      <c r="B3" s="48"/>
       <c r="C3" s="10" t="s">
         <v>11</v>
       </c>
@@ -2334,11 +2574,11 @@
       </c>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="33">
       <c r="A4" s="26">
         <v>12</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="49" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="17" t="s">
@@ -2352,11 +2592,11 @@
       </c>
       <c r="F4" s="25"/>
     </row>
-    <row r="5" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="33">
       <c r="A5" s="26">
         <v>13</v>
       </c>
-      <c r="B5" s="31"/>
+      <c r="B5" s="49"/>
       <c r="C5" s="17" t="s">
         <v>32</v>
       </c>
@@ -2368,11 +2608,11 @@
       </c>
       <c r="F5" s="25"/>
     </row>
-    <row r="6" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="33">
       <c r="A6" s="26">
         <v>15</v>
       </c>
-      <c r="B6" s="31"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="17" t="s">
         <v>34</v>
       </c>
@@ -2384,11 +2624,11 @@
       </c>
       <c r="F6" s="25"/>
     </row>
-    <row r="7" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="33">
       <c r="A7" s="26">
         <v>19</v>
       </c>
-      <c r="B7" s="31"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="17" t="s">
         <v>38</v>
       </c>
@@ -2400,11 +2640,11 @@
       </c>
       <c r="F7" s="25"/>
     </row>
-    <row r="8" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="33">
       <c r="A8" s="26">
         <v>20</v>
       </c>
-      <c r="B8" s="31"/>
+      <c r="B8" s="49"/>
       <c r="C8" s="17" t="s">
         <v>39</v>
       </c>
@@ -2416,11 +2656,11 @@
       </c>
       <c r="F8" s="25"/>
     </row>
-    <row r="9" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="33">
       <c r="A9" s="26">
         <v>21</v>
       </c>
-      <c r="B9" s="31"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="17" t="s">
         <v>40</v>
       </c>
@@ -2432,11 +2672,11 @@
       </c>
       <c r="F9" s="25"/>
     </row>
-    <row r="10" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="33">
       <c r="A10" s="26">
         <v>22</v>
       </c>
-      <c r="B10" s="31"/>
+      <c r="B10" s="49"/>
       <c r="C10" s="17" t="s">
         <v>41</v>
       </c>
@@ -2448,11 +2688,11 @@
       </c>
       <c r="F10" s="25"/>
     </row>
-    <row r="11" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="33">
       <c r="A11" s="26">
         <v>23</v>
       </c>
-      <c r="B11" s="31"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="17" t="s">
         <v>42</v>
       </c>
@@ -2464,11 +2704,11 @@
       </c>
       <c r="F11" s="25"/>
     </row>
-    <row r="12" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="33">
       <c r="A12" s="26">
         <v>24</v>
       </c>
-      <c r="B12" s="31"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="17" t="s">
         <v>43</v>
       </c>
@@ -2480,11 +2720,11 @@
       </c>
       <c r="F12" s="25"/>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="26">
         <v>25</v>
       </c>
-      <c r="B13" s="31"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="21" t="s">
         <v>28</v>
       </c>
@@ -2509,14 +2749,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="48.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -2527,7 +2767,7 @@
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2547,11 +2787,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="21" customHeight="1">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="46" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -2565,11 +2805,11 @@
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="17.25" customHeight="1">
       <c r="A3" s="3">
         <v>3</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="47"/>
       <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
@@ -2581,11 +2821,11 @@
       </c>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="17.25" customHeight="1">
       <c r="A4" s="3">
         <v>6</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="47"/>
       <c r="C4" s="4" t="s">
         <v>15</v>
       </c>
@@ -2597,11 +2837,11 @@
       </c>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="17.25" customHeight="1">
       <c r="A5" s="12">
         <v>8</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="47"/>
       <c r="C5" s="15" t="s">
         <v>12</v>
       </c>
@@ -2613,11 +2853,11 @@
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="66">
       <c r="A6" s="26">
         <v>17</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="49" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -2631,11 +2871,11 @@
       </c>
       <c r="F6" s="25"/>
     </row>
-    <row r="7" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="66">
       <c r="A7" s="26">
         <v>18</v>
       </c>
-      <c r="B7" s="31"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="17" t="s">
         <v>37</v>
       </c>
@@ -2647,11 +2887,11 @@
       </c>
       <c r="F7" s="25"/>
     </row>
-    <row r="8" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="33">
       <c r="A8" s="26">
         <v>27</v>
       </c>
-      <c r="B8" s="31"/>
+      <c r="B8" s="49"/>
       <c r="C8" s="23" t="s">
         <v>45</v>
       </c>
@@ -2663,11 +2903,11 @@
       </c>
       <c r="F8" s="25"/>
     </row>
-    <row r="9" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="33">
       <c r="A9" s="26">
         <v>28</v>
       </c>
-      <c r="B9" s="31"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="16" t="s">
         <v>46</v>
       </c>
@@ -2679,11 +2919,11 @@
       </c>
       <c r="F9" s="25"/>
     </row>
-    <row r="10" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="33">
       <c r="A10" s="26">
         <v>29</v>
       </c>
-      <c r="B10" s="31"/>
+      <c r="B10" s="49"/>
       <c r="C10" s="22" t="s">
         <v>47</v>
       </c>
@@ -2695,11 +2935,11 @@
       </c>
       <c r="F10" s="25"/>
     </row>
-    <row r="11" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="33">
       <c r="A11" s="26">
         <v>30</v>
       </c>
-      <c r="B11" s="31"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="16" t="s">
         <v>48</v>
       </c>
@@ -2711,11 +2951,11 @@
       </c>
       <c r="F11" s="25"/>
     </row>
-    <row r="12" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="33">
       <c r="A12" s="26">
         <v>31</v>
       </c>
-      <c r="B12" s="31"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="17" t="s">
         <v>49</v>
       </c>
@@ -2727,11 +2967,11 @@
       </c>
       <c r="F12" s="25"/>
     </row>
-    <row r="13" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="33">
       <c r="A13" s="26">
         <v>32</v>
       </c>
-      <c r="B13" s="31"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="16" t="s">
         <v>50</v>
       </c>
@@ -2743,11 +2983,11 @@
       </c>
       <c r="F13" s="25"/>
     </row>
-    <row r="14" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="33">
       <c r="A14" s="26">
         <v>33</v>
       </c>
-      <c r="B14" s="31"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="16" t="s">
         <v>51</v>
       </c>
@@ -2759,11 +2999,11 @@
       </c>
       <c r="F14" s="25"/>
     </row>
-    <row r="15" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="33">
       <c r="A15" s="26">
         <v>35</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="49" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="24" t="s">
@@ -2777,11 +3017,11 @@
       </c>
       <c r="F15" s="25"/>
     </row>
-    <row r="16" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="33">
       <c r="A16" s="26">
         <v>36</v>
       </c>
-      <c r="B16" s="31"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="7" t="s">
         <v>54</v>
       </c>
@@ -2793,11 +3033,11 @@
       </c>
       <c r="F16" s="25"/>
     </row>
-    <row r="17" spans="1:6" ht="33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="33">
       <c r="A17" s="26">
         <v>37</v>
       </c>
-      <c r="B17" s="31"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="7" t="s">
         <v>55</v>
       </c>
@@ -2817,4 +3057,423 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" style="28"/>
+    <col min="3" max="3" width="22" style="28" customWidth="1"/>
+    <col min="4" max="4" width="90.7109375" style="40" customWidth="1"/>
+    <col min="5" max="5" width="44" style="33" customWidth="1"/>
+    <col min="6" max="6" width="29" style="40" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" style="44" customWidth="1"/>
+    <col min="8" max="8" width="53.42578125" style="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" s="28" customFormat="1">
+      <c r="D1" s="38"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="35"/>
+    </row>
+    <row r="2" spans="2:8">
+      <c r="B2" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="41"/>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="B3" s="53">
+        <v>1</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="42"/>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="54"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="42"/>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="54"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="42"/>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" s="54"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="42"/>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" s="54"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="42"/>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" s="54"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="42"/>
+    </row>
+    <row r="9" spans="2:8" ht="31.5">
+      <c r="B9" s="54"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="66" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="63" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" s="42"/>
+    </row>
+    <row r="10" spans="2:8" ht="31.5">
+      <c r="B10" s="54"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="63" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="45">
+      <c r="B11" s="54"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="43" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="15.75">
+      <c r="B12" s="54"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="63" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="15.75">
+      <c r="B13" s="54"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" s="63" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="15.75">
+      <c r="B14" s="54"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="60" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="63" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="15.75">
+      <c r="B15" s="54"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="64" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="63" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="15.75">
+      <c r="B16" s="54"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="60" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="63" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15.75">
+      <c r="B17" s="54"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="63" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="54"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="54"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19" s="43" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" s="54"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" s="54"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" s="43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" s="55"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G22" s="43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" s="56"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="36"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="56"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="59" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="56"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="58" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="D26" s="58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:C22"/>
+    <mergeCell ref="B3:B22"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D15" r:id="rId1" location="hasVippieNumber(java.util.List)" display="C:\Users\HoangNam\Documents\doc\unique\packagename\sdkwrapper\contacts\ContactsWrapper.html - hasVippieNumber(java.util.List)"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>